<commit_message>
Modificaciones en plantilla para subir productos
</commit_message>
<xml_diff>
--- a/public/formats/co-items.xlsx
+++ b/public/formats/co-items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Código Interno</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Codigo Tipo de Impuesto Compra</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Talla</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -418,7 +424,7 @@
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -455,8 +461,14 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -493,8 +505,14 @@
       <c r="L2" t="s">
         <v>14</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -530,6 +548,12 @@
       </c>
       <c r="L3" t="s">
         <v>15</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>